<commit_message>
Readme + upload project
</commit_message>
<xml_diff>
--- a/creditCards.xlsx
+++ b/creditCards.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f6ed943d1b60755/Desktop/Pyhton/final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_DB74287A773F03F9F99B5F4B46741F10AD6662F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{525AAD92-44A5-4022-9147-2269FFF8DB37}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_DB74287A773F03F9F99B5F4B46741F10AD6662F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF2BCAAD-91B4-4545-B8D4-A463FA4C29C6}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="1590" windowWidth="13830" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="645" yWindow="1800" windowWidth="13830" windowHeight="13680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
     <sheet name="2" sheetId="2" r:id="rId2"/>
     <sheet name="3" sheetId="3" r:id="rId3"/>
+    <sheet name="4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -73,6 +74,12 @@
   </si>
   <si>
     <t>RO49AAAA1B31007593840000</t>
+  </si>
+  <si>
+    <t>Anne Proust</t>
+  </si>
+  <si>
+    <t>RON12KRO03959105014</t>
   </si>
 </sst>
 </file>
@@ -185,6 +192,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -452,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,7 +797,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,4 +1038,83 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9F2E55E-63E0-4318-893C-3D1498AF22AC}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>44849</v>
+      </c>
+      <c r="B4" s="9">
+        <v>2425</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>44851</v>
+      </c>
+      <c r="B5" s="9">
+        <v>500</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>44851</v>
+      </c>
+      <c r="B6" s="9">
+        <v>-230</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>